<commit_message>
Added: Fields for hours
</commit_message>
<xml_diff>
--- a/Presupuesto.xlsx
+++ b/Presupuesto.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vale-\GSNSF-DELSAVIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822FC08A-E400-4DE4-BACA-764F918277A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{154E9302-FABF-4B3C-8703-874150B59326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0E17E260-4916-4B14-8CC2-3EC561FC2622}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dominio y Hosting" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculadora" sheetId="2" r:id="rId1"/>
+    <sheet name="Dominio y Hosting" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +32,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Precio hora</t>
+  </si>
+  <si>
+    <t>Horas de diseño</t>
+  </si>
+  <si>
+    <t>Horas de prototipado</t>
+  </si>
+  <si>
+    <t>Horas de desarrollo</t>
+  </si>
+  <si>
+    <t>Horas de prueba</t>
+  </si>
+  <si>
+    <t>Horas de subida</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,10 +403,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8CBE16-A1BF-479E-A773-F6E067ED2ED0}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA8B141-BF6D-4361-B4AC-2BE8940BB551}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -391,21 +463,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002BE8710E5985B4B856B7533B5474BF7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56f6d7ce4f3a8b0ba88435d7548e75e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="84c67e9b-7343-4ac1-a15f-e9392c2a3db9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03198ca8b3cfee05c9e46239ccfb4cae" ns3:_="">
     <xsd:import namespace="84c67e9b-7343-4ac1-a15f-e9392c2a3db9"/>
@@ -561,31 +618,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1BAB8D-6679-4A77-9207-1BB48642EEB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="84c67e9b-7343-4ac1-a15f-e9392c2a3db9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CF309B-E78A-418C-A5D9-27CD6E86A84C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E130D7DA-87A8-48EE-8EBB-9DD2A5A78219}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -601,4 +649,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1BAB8D-6679-4A77-9207-1BB48642EEB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="84c67e9b-7343-4ac1-a15f-e9392c2a3db9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CF309B-E78A-418C-A5D9-27CD6E86A84C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>